<commit_message>
add DOM clobbering into HTML injection test
</commit_message>
<xml_diff>
--- a/Secure D Web Application Security Test Checklist v1.00.xlsx
+++ b/Secure D Web Application Security Test Checklist v1.00.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bankde/Desktop/work/wastc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6EAF45-AA16-ED4D-B956-FE124342F4E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A43B1F-3A05-3F47-82C0-E7BE5E0140D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project information" sheetId="1" r:id="rId1"/>
@@ -1052,11 +1052,6 @@
 - Tools: OWASP ZAP, nikto, manual review</t>
   </si>
   <si>
-    <t>- While not as critical as XSS, allowing HTML structure injection gives attacker ability to insert malicious contents or redirect traffic to malicious site.
-- Test with HTML tags: &lt;form&gt; &lt;a href&gt; &lt;iframe&gt;
-- Tools: OWASP ZAP, nikto, manual review</t>
-  </si>
-  <si>
     <t>- Web application written with c, c++
 - Using vulnerable programming language versions of Python, NodeJS, etc.
 - Test by long, gibberish input
@@ -3003,6 +2998,12 @@
   </si>
   <si>
     <t>Secure D Web Application Security Test Checklist v1.00</t>
+  </si>
+  <si>
+    <t>- While not as critical as XSS, allowing HTML structure injection gives attacker ability to insert malicious contents or redirect traffic to malicious site.
+- Test with HTML tags: &lt;form&gt; &lt;a href&gt; &lt;iframe&gt;
+- Try DOM Clobbering for possible XSS
+- Tools: OWASP ZAP, nikto, manual review</t>
   </si>
 </sst>
 </file>
@@ -4489,7 +4490,7 @@
   </sheetPr>
   <dimension ref="A1:IV8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -4546,7 +4547,7 @@
     <row r="8" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5"/>
       <c r="B8" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -4699,7 +4700,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -4772,15 +4773,15 @@
         <v>9</v>
       </c>
       <c r="B13" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>255</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>256</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -4899,15 +4900,15 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>238</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>239</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="84" x14ac:dyDescent="0.15">
@@ -4934,24 +4935,24 @@
         <v>37</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A9" s="14"/>
       <c r="B9" s="26"/>
       <c r="C9" s="22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="154" x14ac:dyDescent="0.15">
@@ -5026,7 +5027,7 @@
         <v>46</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
@@ -5038,7 +5039,7 @@
       <c r="A15" s="14"/>
       <c r="B15" s="26"/>
       <c r="C15" s="22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -5102,7 +5103,7 @@
         <v>53</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -5114,7 +5115,7 @@
       <c r="A20" s="27"/>
       <c r="B20" s="23"/>
       <c r="C20" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
@@ -5246,7 +5247,7 @@
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="126" x14ac:dyDescent="0.15">
@@ -5257,7 +5258,7 @@
         <v>61</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="17"/>
@@ -5269,7 +5270,7 @@
       <c r="A6" s="20"/>
       <c r="B6" s="26"/>
       <c r="C6" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -5281,7 +5282,7 @@
       <c r="A7" s="20"/>
       <c r="B7" s="26"/>
       <c r="C7" s="22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -5297,7 +5298,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -5309,7 +5310,7 @@
       <c r="A9" s="20"/>
       <c r="B9" s="26"/>
       <c r="C9" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -5321,7 +5322,7 @@
       <c r="A10" s="20"/>
       <c r="B10" s="26"/>
       <c r="C10" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -5333,7 +5334,7 @@
       <c r="A11" s="20"/>
       <c r="B11" s="26"/>
       <c r="C11" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -5345,7 +5346,7 @@
       <c r="A12" s="20"/>
       <c r="B12" s="26"/>
       <c r="C12" s="22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -5425,7 +5426,7 @@
         <v>78</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -5437,19 +5438,19 @@
       <c r="A18" s="20"/>
       <c r="B18" s="26"/>
       <c r="C18" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="84" x14ac:dyDescent="0.15">
       <c r="A19" s="20"/>
       <c r="B19" s="26"/>
       <c r="C19" s="22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -5465,7 +5466,7 @@
         <v>80</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
@@ -5477,7 +5478,7 @@
       <c r="A21" s="20"/>
       <c r="B21" s="26"/>
       <c r="C21" s="22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -5489,19 +5490,19 @@
       <c r="A22" s="20"/>
       <c r="B22" s="26"/>
       <c r="C22" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="56" x14ac:dyDescent="0.15">
       <c r="A23" s="20"/>
       <c r="B23" s="26"/>
       <c r="C23" s="22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -5517,7 +5518,7 @@
         <v>84</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
@@ -5529,7 +5530,7 @@
       <c r="A25" s="20"/>
       <c r="B25" s="26"/>
       <c r="C25" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
@@ -5545,7 +5546,7 @@
         <v>87</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
@@ -5582,7 +5583,7 @@
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
       <c r="F28" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="126" x14ac:dyDescent="0.15">
@@ -5598,7 +5599,7 @@
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="70" x14ac:dyDescent="0.15">
@@ -5653,7 +5654,7 @@
   </sheetPr>
   <dimension ref="A1:IV33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -5720,12 +5721,12 @@
         <v>99</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="140" x14ac:dyDescent="0.15">
@@ -5784,7 +5785,7 @@
         <v>106</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -5816,7 +5817,7 @@
         <v>109</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -5832,19 +5833,19 @@
         <v>111</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A12" s="20"/>
       <c r="B12" s="26"/>
       <c r="C12" s="22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -5856,7 +5857,7 @@
       <c r="A13" s="20"/>
       <c r="B13" s="26"/>
       <c r="C13" s="22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
@@ -5904,7 +5905,7 @@
         <v>117</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>231</v>
+        <v>303</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
@@ -5920,7 +5921,7 @@
         <v>118</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -5936,7 +5937,7 @@
         <v>120</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -5968,7 +5969,7 @@
         <v>123</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
@@ -5984,7 +5985,7 @@
         <v>125</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -6000,7 +6001,7 @@
         <v>127</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
@@ -6013,15 +6014,15 @@
         <v>17</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
       <c r="F23" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="112" x14ac:dyDescent="0.15">
@@ -6032,7 +6033,7 @@
         <v>129</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
@@ -6048,7 +6049,7 @@
         <v>131</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
@@ -6064,7 +6065,7 @@
         <v>133</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
@@ -6080,7 +6081,7 @@
         <v>135</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
@@ -6096,7 +6097,7 @@
         <v>137</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
@@ -6279,7 +6280,7 @@
         <v>147</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -6454,7 +6455,7 @@
         <v>160</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -6470,12 +6471,12 @@
         <v>162</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="70" x14ac:dyDescent="0.15">
@@ -6486,7 +6487,7 @@
         <v>163</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -6499,15 +6500,15 @@
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28" x14ac:dyDescent="0.15">
@@ -6515,15 +6516,15 @@
         <v>6</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="42" x14ac:dyDescent="0.15">
@@ -6550,7 +6551,7 @@
         <v>167</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>

</xml_diff>

<commit_message>
add Information Disclosure - Insecure config 3rd party service
</commit_message>
<xml_diff>
--- a/Secure D Web Application Security Test Checklist v1.00.xlsx
+++ b/Secure D Web Application Security Test Checklist v1.00.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bankde/Desktop/work/wastc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A43B1F-3A05-3F47-82C0-E7BE5E0140D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1CBF68-3B60-A147-B651-6268B5430610}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project information" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="307">
   <si>
     <t>Project Information</t>
   </si>
@@ -146,9 +146,6 @@
   </si>
   <si>
     <t>Insecure caching</t>
-  </si>
-  <si>
-    <t>Insecure usage of web storage</t>
   </si>
   <si>
     <t>[CWE-312, CWE-922]
@@ -3004,6 +3001,23 @@
 - Test with HTML tags: &lt;form&gt; &lt;a href&gt; &lt;iframe&gt;
 - Try DOM Clobbering for possible XSS
 - Tools: OWASP ZAP, nikto, manual review</t>
+  </si>
+  <si>
+    <t>Insecure usage of browser local storage</t>
+  </si>
+  <si>
+    <t>Insecure configuration of 3rd party services</t>
+  </si>
+  <si>
+    <t>- Incorrect ACL or privilege policy on 3rd party storage.
+    - Amazon (s3)
+    - Firebase database
+- Missing authorization control when using callback service
+    - LINE chatbot
+    - Dialogflow</t>
+  </si>
+  <si>
+    <t>The developer should review the security best practice guideline on each service that is integrated into the application.</t>
   </si>
 </sst>
 </file>
@@ -4547,7 +4561,7 @@
     <row r="8" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5"/>
       <c r="B8" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -4573,7 +4587,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4636,7 +4650,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
@@ -4649,10 +4663,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>170</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>171</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -4668,7 +4682,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -4684,7 +4698,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -4700,7 +4714,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -4716,7 +4730,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -4744,12 +4758,12 @@
         <v>26</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="42" x14ac:dyDescent="0.15">
@@ -4760,7 +4774,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -4773,15 +4787,15 @@
         <v>9</v>
       </c>
       <c r="B13" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>254</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>255</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -4802,13 +4816,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV22"/>
+  <dimension ref="A1:IV23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4871,7 +4885,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
@@ -4887,7 +4901,7 @@
         <v>33</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -4900,15 +4914,15 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>237</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>238</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="84" x14ac:dyDescent="0.15">
@@ -4919,7 +4933,7 @@
         <v>35</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -4935,24 +4949,24 @@
         <v>37</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A9" s="14"/>
       <c r="B9" s="26"/>
       <c r="C9" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="154" x14ac:dyDescent="0.15">
@@ -4960,15 +4974,15 @@
         <v>6</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>38</v>
+        <v>303</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="112" x14ac:dyDescent="0.15">
@@ -4976,15 +4990,15 @@
         <v>7</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="98" x14ac:dyDescent="0.15">
@@ -4992,15 +5006,15 @@
         <v>8</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="140" x14ac:dyDescent="0.15">
@@ -5008,15 +5022,15 @@
         <v>9</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="98" x14ac:dyDescent="0.15">
@@ -5024,27 +5038,27 @@
         <v>10</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="154" x14ac:dyDescent="0.15">
       <c r="A15" s="14"/>
       <c r="B15" s="26"/>
       <c r="C15" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="140" x14ac:dyDescent="0.15">
@@ -5052,15 +5066,15 @@
         <v>11</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="84" x14ac:dyDescent="0.15">
@@ -5068,15 +5082,15 @@
         <v>12</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="56" x14ac:dyDescent="0.15">
@@ -5084,15 +5098,15 @@
         <v>13</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="70" x14ac:dyDescent="0.15">
@@ -5100,27 +5114,27 @@
         <v>14</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A20" s="27"/>
       <c r="B20" s="23"/>
       <c r="C20" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="306" x14ac:dyDescent="0.15">
@@ -5128,15 +5142,15 @@
         <v>15</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
       <c r="F21" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="70" x14ac:dyDescent="0.15">
@@ -5144,15 +5158,31 @@
         <v>16</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="84" x14ac:dyDescent="0.15">
+      <c r="A23" s="14">
+        <v>17</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="18" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -5196,7 +5226,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A1" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -5206,7 +5236,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -5239,15 +5269,15 @@
         <v>1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="28" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="126" x14ac:dyDescent="0.15">
@@ -5255,39 +5285,39 @@
         <v>2</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="17"/>
       <c r="F5" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A6" s="20"/>
       <c r="B6" s="26"/>
       <c r="C6" s="22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="98" x14ac:dyDescent="0.15">
       <c r="A7" s="20"/>
       <c r="B7" s="26"/>
       <c r="C7" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="140" x14ac:dyDescent="0.15">
@@ -5295,63 +5325,63 @@
         <v>3</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A9" s="20"/>
       <c r="B9" s="26"/>
       <c r="C9" s="22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="98" x14ac:dyDescent="0.15">
       <c r="A10" s="20"/>
       <c r="B10" s="26"/>
       <c r="C10" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="56" x14ac:dyDescent="0.15">
       <c r="A11" s="20"/>
       <c r="B11" s="26"/>
       <c r="C11" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="56" x14ac:dyDescent="0.15">
       <c r="A12" s="20"/>
       <c r="B12" s="26"/>
       <c r="C12" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="98" x14ac:dyDescent="0.15">
@@ -5359,15 +5389,15 @@
         <v>4</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="70" x14ac:dyDescent="0.15">
@@ -5375,15 +5405,15 @@
         <v>5</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="42" x14ac:dyDescent="0.15">
@@ -5391,15 +5421,15 @@
         <v>6</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="70" x14ac:dyDescent="0.15">
@@ -5407,15 +5437,15 @@
         <v>7</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="154" x14ac:dyDescent="0.15">
@@ -5423,39 +5453,39 @@
         <v>8</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A18" s="20"/>
       <c r="B18" s="26"/>
       <c r="C18" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="84" x14ac:dyDescent="0.15">
       <c r="A19" s="20"/>
       <c r="B19" s="26"/>
       <c r="C19" s="22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="140" x14ac:dyDescent="0.15">
@@ -5463,51 +5493,51 @@
         <v>9</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A21" s="20"/>
       <c r="B21" s="26"/>
       <c r="C21" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
       <c r="F21" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="112" x14ac:dyDescent="0.15">
       <c r="A22" s="20"/>
       <c r="B22" s="26"/>
       <c r="C22" s="22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="56" x14ac:dyDescent="0.15">
       <c r="A23" s="20"/>
       <c r="B23" s="26"/>
       <c r="C23" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
       <c r="F23" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="126" x14ac:dyDescent="0.15">
@@ -5515,27 +5545,27 @@
         <v>10</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
       <c r="F24" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A25" s="20"/>
       <c r="B25" s="26"/>
       <c r="C25" s="22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
       <c r="F25" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="56" x14ac:dyDescent="0.15">
@@ -5543,15 +5573,15 @@
         <v>11</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
       <c r="F26" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="112" x14ac:dyDescent="0.15">
@@ -5559,15 +5589,15 @@
         <v>12</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="112" x14ac:dyDescent="0.15">
@@ -5575,15 +5605,15 @@
         <v>13</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
       <c r="F28" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="126" x14ac:dyDescent="0.15">
@@ -5591,15 +5621,15 @@
         <v>14</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="70" x14ac:dyDescent="0.15">
@@ -5607,15 +5637,15 @@
         <v>15</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
       <c r="F30" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="84" x14ac:dyDescent="0.15">
@@ -5623,15 +5653,15 @@
         <v>16</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
       <c r="F31" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -5654,11 +5684,11 @@
   </sheetPr>
   <dimension ref="A1:IV33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5675,7 +5705,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A1" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -5685,7 +5715,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -5718,15 +5748,15 @@
         <v>1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="140" x14ac:dyDescent="0.15">
@@ -5734,15 +5764,15 @@
         <v>2</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="182" x14ac:dyDescent="0.15">
@@ -5750,15 +5780,15 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="126" x14ac:dyDescent="0.15">
@@ -5766,15 +5796,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="126" x14ac:dyDescent="0.15">
@@ -5782,15 +5812,15 @@
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="293" x14ac:dyDescent="0.15">
@@ -5798,15 +5828,15 @@
         <v>6</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="182" x14ac:dyDescent="0.15">
@@ -5814,15 +5844,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="112" x14ac:dyDescent="0.15">
@@ -5830,39 +5860,39 @@
         <v>8</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A12" s="20"/>
       <c r="B12" s="26"/>
       <c r="C12" s="22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="84" x14ac:dyDescent="0.15">
       <c r="A13" s="20"/>
       <c r="B13" s="26"/>
       <c r="C13" s="22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="126" x14ac:dyDescent="0.15">
@@ -5870,15 +5900,15 @@
         <v>9</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="332" x14ac:dyDescent="0.15">
@@ -5886,15 +5916,15 @@
         <v>9</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="154" x14ac:dyDescent="0.15">
@@ -5902,15 +5932,15 @@
         <v>10</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="98" x14ac:dyDescent="0.15">
@@ -5918,15 +5948,15 @@
         <v>11</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="84" x14ac:dyDescent="0.15">
@@ -5934,15 +5964,15 @@
         <v>12</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="168" x14ac:dyDescent="0.15">
@@ -5950,15 +5980,15 @@
         <v>13</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="168" x14ac:dyDescent="0.15">
@@ -5966,15 +5996,15 @@
         <v>14</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="196" x14ac:dyDescent="0.15">
@@ -5982,15 +6012,15 @@
         <v>15</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
       <c r="F21" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="210" x14ac:dyDescent="0.15">
@@ -5998,15 +6028,15 @@
         <v>16</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="84" x14ac:dyDescent="0.15">
@@ -6014,15 +6044,15 @@
         <v>17</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
       <c r="F23" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="112" x14ac:dyDescent="0.15">
@@ -6030,15 +6060,15 @@
         <v>18</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
       <c r="F24" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="98" x14ac:dyDescent="0.15">
@@ -6046,15 +6076,15 @@
         <v>19</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
       <c r="F25" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="98" x14ac:dyDescent="0.15">
@@ -6062,15 +6092,15 @@
         <v>20</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
       <c r="F26" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="98" x14ac:dyDescent="0.15">
@@ -6078,15 +6108,15 @@
         <v>21</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="140" x14ac:dyDescent="0.15">
@@ -6094,15 +6124,15 @@
         <v>22</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
       <c r="F28" s="24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="210" x14ac:dyDescent="0.15">
@@ -6110,15 +6140,15 @@
         <v>23</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="112" x14ac:dyDescent="0.15">
@@ -6126,15 +6156,15 @@
         <v>24</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
       <c r="F30" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="70" x14ac:dyDescent="0.15">
@@ -6142,39 +6172,39 @@
         <v>25</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
       <c r="F31" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A32" s="20"/>
       <c r="B32" s="26"/>
       <c r="C32" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="17"/>
       <c r="F32" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="84" x14ac:dyDescent="0.15">
       <c r="A33" s="20"/>
       <c r="B33" s="26"/>
       <c r="C33" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D33" s="17"/>
       <c r="E33" s="17"/>
       <c r="F33" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -6218,7 +6248,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -6228,7 +6258,7 @@
     </row>
     <row r="2" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -6261,15 +6291,15 @@
         <v>1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="345" x14ac:dyDescent="0.15">
@@ -6277,15 +6307,15 @@
         <v>2</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="84" x14ac:dyDescent="0.15">
@@ -6293,15 +6323,15 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="112" x14ac:dyDescent="0.15">
@@ -6309,15 +6339,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="84" x14ac:dyDescent="0.15">
@@ -6325,15 +6355,15 @@
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="70" x14ac:dyDescent="0.15">
@@ -6341,15 +6371,15 @@
         <v>6</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -6393,7 +6423,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A1" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -6403,7 +6433,7 @@
     </row>
     <row r="2" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -6436,15 +6466,15 @@
         <v>1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="42" x14ac:dyDescent="0.15">
@@ -6452,15 +6482,15 @@
         <v>2</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="56" x14ac:dyDescent="0.15">
@@ -6468,15 +6498,15 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="70" x14ac:dyDescent="0.15">
@@ -6484,15 +6514,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.15">
@@ -6500,15 +6530,15 @@
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28" x14ac:dyDescent="0.15">
@@ -6516,15 +6546,15 @@
         <v>6</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="42" x14ac:dyDescent="0.15">
@@ -6532,15 +6562,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="56" x14ac:dyDescent="0.15">
@@ -6548,15 +6578,15 @@
         <v>8</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add note on arbitrage opportunity
</commit_message>
<xml_diff>
--- a/Secure D Web Application Security Test Checklist v1.00.xlsx
+++ b/Secure D Web Application Security Test Checklist v1.00.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bankde/Desktop/work/wastc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF272C62-841C-0947-AA6E-C194ADC8152A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C57E0C-E396-744A-B6FC-B3DA35007968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project information" sheetId="1" r:id="rId1"/>
@@ -787,13 +787,6 @@
 - Unable to counter repudiation from malicious users.
 - Unable to mitigate and prevent on-going vulnerable application.
 - Should consist of: Who doing what where how when</t>
-  </si>
-  <si>
-    <t>- Improper money exchange rate. 
-Such as getting small sum from trading A -&gt; B -&gt; C -&gt; A
-- Repeatable of discount, reward, voucher or gift.
-- Game with rewards or leaderboard from repetitive tasks (thus, vulnerable to bot) or client-side logic.
-- Signup reward of unauthenticated registration.</t>
   </si>
   <si>
     <t>- Phishing attack or confusion cause from the similarity in different unicode characters. (E.g. English, Latin, Greek, Cyrillic, etc)
@@ -3003,6 +2996,13 @@
         - nsec3map
 - Internet wide scan data project
     - Forward DNS dataset (Project Sonar)</t>
+  </si>
+  <si>
+    <t>- Improper money exchange rate. (Arbitrage opportunity)
+Such as getting small sum from trading A -&gt; B -&gt; C -&gt; A
+- Repeatable of discount, reward, voucher or gift.
+- Game with rewards or leaderboard from repetitive tasks (thus, vulnerable to bot) or client-side logic.
+- Signup reward of unauthenticated registration.</t>
   </si>
 </sst>
 </file>
@@ -3378,15 +3378,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -3410,6 +3401,15 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4573,8 +4573,8 @@
   </sheetPr>
   <dimension ref="A1:IV8"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4586,10 +4586,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="40"/>
     </row>
     <row r="2" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
@@ -4630,7 +4630,7 @@
     <row r="8" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5"/>
       <c r="B8" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -4652,11 +4652,11 @@
   </sheetPr>
   <dimension ref="A1:IW13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4664,7 +4664,7 @@
     <col min="1" max="1" width="4.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="46" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" style="39" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" style="36" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="1" customWidth="1"/>
     <col min="7" max="7" width="42.33203125" style="1" customWidth="1"/>
@@ -4673,26 +4673,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
@@ -4705,7 +4705,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -4725,10 +4725,10 @@
         <v>15</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="D4" s="35" t="s">
         <v>269</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>270</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -4744,10 +4744,10 @@
         <v>168</v>
       </c>
       <c r="C5" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>271</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>272</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -4763,10 +4763,10 @@
         <v>17</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="D6" s="37" t="s">
         <v>273</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>272</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -4782,10 +4782,10 @@
         <v>18</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>276</v>
-      </c>
-      <c r="D7" s="37" t="s">
         <v>275</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>274</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
@@ -4801,10 +4801,10 @@
         <v>20</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>278</v>
-      </c>
-      <c r="D8" s="37" t="s">
         <v>277</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>276</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -4820,10 +4820,10 @@
         <v>22</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
@@ -4837,7 +4837,7 @@
       <c r="C10" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="34" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="17"/>
@@ -4854,7 +4854,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>169</v>
@@ -4873,10 +4873,10 @@
         <v>27</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>281</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>270</v>
+        <v>280</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>269</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
@@ -4889,18 +4889,18 @@
         <v>9</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="D13" s="37" t="s">
         <v>283</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>282</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
       <c r="G13" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -4944,26 +4944,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
@@ -4976,7 +4976,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -4996,10 +4996,10 @@
         <v>31</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -5015,10 +5015,10 @@
         <v>33</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -5031,10 +5031,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>209</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>210</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>16</v>
@@ -5042,7 +5042,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="84" x14ac:dyDescent="0.15">
@@ -5072,22 +5072,22 @@
         <v>37</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="70" x14ac:dyDescent="0.15">
       <c r="A9" s="14"/>
       <c r="B9" s="26"/>
       <c r="C9" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>16</v>
@@ -5095,7 +5095,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="154" x14ac:dyDescent="0.15">
@@ -5103,12 +5103,12 @@
         <v>6</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>289</v>
-      </c>
-      <c r="D10" s="40" t="s">
+        <v>288</v>
+      </c>
+      <c r="D10" s="37" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="17"/>
@@ -5125,9 +5125,9 @@
         <v>39</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="D11" s="40" t="s">
+        <v>289</v>
+      </c>
+      <c r="D11" s="37" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="17"/>
@@ -5144,9 +5144,9 @@
         <v>41</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>291</v>
-      </c>
-      <c r="D12" s="40" t="s">
+        <v>290</v>
+      </c>
+      <c r="D12" s="37" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="17"/>
@@ -5163,10 +5163,10 @@
         <v>43</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -5182,10 +5182,10 @@
         <v>45</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>294</v>
-      </c>
-      <c r="D14" s="40" t="s">
         <v>293</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>292</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
@@ -5197,10 +5197,10 @@
       <c r="A15" s="14"/>
       <c r="B15" s="26"/>
       <c r="C15" s="22" t="s">
-        <v>296</v>
-      </c>
-      <c r="D15" s="40" t="s">
         <v>295</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>294</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
@@ -5216,10 +5216,10 @@
         <v>47</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
@@ -5235,10 +5235,10 @@
         <v>48</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
@@ -5254,10 +5254,10 @@
         <v>50</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -5273,10 +5273,10 @@
         <v>52</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -5288,9 +5288,9 @@
       <c r="A20" s="27"/>
       <c r="B20" s="23"/>
       <c r="C20" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="D20" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="D20" s="37" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="17"/>
@@ -5307,10 +5307,10 @@
         <v>54</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>302</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>270</v>
+        <v>301</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>269</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
@@ -5326,10 +5326,10 @@
         <v>55</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
@@ -5342,18 +5342,18 @@
         <v>17</v>
       </c>
       <c r="B23" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="37" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -5380,7 +5380,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5397,26 +5397,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
@@ -5429,7 +5429,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -5451,13 +5451,13 @@
       <c r="C4" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="126" x14ac:dyDescent="0.15">
@@ -5468,9 +5468,9 @@
         <v>60</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="D5" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="D5" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="12"/>
@@ -5483,9 +5483,9 @@
       <c r="A6" s="20"/>
       <c r="B6" s="26"/>
       <c r="C6" s="22" t="s">
-        <v>235</v>
-      </c>
-      <c r="D6" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="17"/>
@@ -5498,9 +5498,9 @@
       <c r="A7" s="20"/>
       <c r="B7" s="26"/>
       <c r="C7" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="D7" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="17"/>
@@ -5517,9 +5517,9 @@
         <v>63</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>237</v>
-      </c>
-      <c r="D8" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="17"/>
@@ -5532,9 +5532,9 @@
       <c r="A9" s="20"/>
       <c r="B9" s="26"/>
       <c r="C9" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="D9" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="17"/>
@@ -5547,9 +5547,9 @@
       <c r="A10" s="20"/>
       <c r="B10" s="26"/>
       <c r="C10" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="D10" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="17"/>
@@ -5562,9 +5562,9 @@
       <c r="A11" s="20"/>
       <c r="B11" s="26"/>
       <c r="C11" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="D11" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="17"/>
@@ -5577,9 +5577,9 @@
       <c r="A12" s="20"/>
       <c r="B12" s="26"/>
       <c r="C12" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="D12" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="D12" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="17"/>
@@ -5596,9 +5596,9 @@
         <v>69</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="D13" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="D13" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="17"/>
@@ -5615,9 +5615,9 @@
         <v>71</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="D14" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="D14" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="17"/>
@@ -5636,7 +5636,7 @@
       <c r="C15" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="17"/>
@@ -5655,7 +5655,7 @@
       <c r="C16" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="17"/>
@@ -5672,9 +5672,9 @@
         <v>77</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="D17" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="D17" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="17"/>
@@ -5687,24 +5687,24 @@
       <c r="A18" s="20"/>
       <c r="B18" s="26"/>
       <c r="C18" s="22" t="s">
-        <v>243</v>
-      </c>
-      <c r="D18" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="D18" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="84" x14ac:dyDescent="0.15">
       <c r="A19" s="20"/>
       <c r="B19" s="26"/>
       <c r="C19" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="D19" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="D19" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="17"/>
@@ -5721,9 +5721,9 @@
         <v>79</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="D20" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="D20" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="17"/>
@@ -5736,9 +5736,9 @@
       <c r="A21" s="20"/>
       <c r="B21" s="26"/>
       <c r="C21" s="22" t="s">
-        <v>247</v>
-      </c>
-      <c r="D21" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="D21" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="17"/>
@@ -5751,24 +5751,24 @@
       <c r="A22" s="20"/>
       <c r="B22" s="26"/>
       <c r="C22" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="D22" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D22" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="56" x14ac:dyDescent="0.15">
       <c r="A23" s="20"/>
       <c r="B23" s="26"/>
       <c r="C23" s="22" t="s">
-        <v>250</v>
-      </c>
-      <c r="D23" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="D23" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="17"/>
@@ -5785,9 +5785,9 @@
         <v>83</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="D24" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="D24" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="17"/>
@@ -5800,9 +5800,9 @@
       <c r="A25" s="20"/>
       <c r="B25" s="26"/>
       <c r="C25" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="D25" s="35" t="s">
+        <v>251</v>
+      </c>
+      <c r="D25" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E25" s="17"/>
@@ -5819,9 +5819,9 @@
         <v>86</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="D26" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="D26" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="17"/>
@@ -5840,7 +5840,7 @@
       <c r="C27" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E27" s="17"/>
@@ -5859,13 +5859,13 @@
       <c r="C28" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
       <c r="G28" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="126" x14ac:dyDescent="0.15">
@@ -5878,13 +5878,13 @@
       <c r="C29" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
       <c r="G29" s="24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="70" x14ac:dyDescent="0.15">
@@ -5897,7 +5897,7 @@
       <c r="C30" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="17"/>
@@ -5916,7 +5916,7 @@
       <c r="C31" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D31" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E31" s="17"/>
@@ -5966,26 +5966,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
@@ -5998,7 +5998,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -6018,15 +6018,15 @@
         <v>98</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="D4" s="35" t="s">
         <v>305</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>304</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="126" x14ac:dyDescent="0.15">
@@ -6037,10 +6037,10 @@
         <v>99</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>308</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>304</v>
+        <v>307</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>303</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -6056,10 +6056,10 @@
         <v>101</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>307</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>304</v>
+        <v>306</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>303</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -6075,10 +6075,10 @@
         <v>103</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>309</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>304</v>
+        <v>308</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>303</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
@@ -6094,10 +6094,10 @@
         <v>105</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>310</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>304</v>
+        <v>309</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>303</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -6113,10 +6113,10 @@
         <v>107</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>304</v>
+        <v>310</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>303</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
@@ -6132,9 +6132,9 @@
         <v>108</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="D10" s="36"/>
+        <v>255</v>
+      </c>
+      <c r="D10" s="33"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="18" t="s">
@@ -6149,24 +6149,24 @@
         <v>110</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>312</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>304</v>
+        <v>311</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>303</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="70" x14ac:dyDescent="0.15">
       <c r="A12" s="20"/>
       <c r="B12" s="26"/>
       <c r="C12" s="22" t="s">
-        <v>258</v>
-      </c>
-      <c r="D12" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="D12" s="39" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="17"/>
@@ -6179,10 +6179,10 @@
       <c r="A13" s="20"/>
       <c r="B13" s="26"/>
       <c r="C13" s="22" t="s">
-        <v>313</v>
-      </c>
-      <c r="D13" s="42" t="s">
-        <v>304</v>
+        <v>312</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>303</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -6200,7 +6200,7 @@
       <c r="C14" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="33" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="17"/>
@@ -6217,10 +6217,10 @@
         <v>115</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>314</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>304</v>
+        <v>313</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>303</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
@@ -6236,10 +6236,10 @@
         <v>116</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>304</v>
+        <v>314</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>303</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
@@ -6255,9 +6255,9 @@
         <v>117</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>259</v>
-      </c>
-      <c r="D17" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="33" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="17"/>
@@ -6274,10 +6274,10 @@
         <v>119</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>316</v>
-      </c>
-      <c r="D18" s="42" t="s">
-        <v>304</v>
+        <v>315</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>303</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -6293,10 +6293,10 @@
         <v>121</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>317</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>304</v>
+        <v>316</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>303</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -6312,9 +6312,9 @@
         <v>122</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="D20" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="D20" s="33" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="17"/>
@@ -6331,9 +6331,9 @@
         <v>124</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="D21" s="36" t="s">
+        <v>207</v>
+      </c>
+      <c r="D21" s="33" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="17"/>
@@ -6350,9 +6350,9 @@
         <v>126</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="D22" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="D22" s="33" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="17"/>
@@ -6366,18 +6366,18 @@
         <v>17</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="D23" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="D23" s="33" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="98" x14ac:dyDescent="0.15">
@@ -6388,10 +6388,10 @@
         <v>128</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>318</v>
-      </c>
-      <c r="D24" s="42" t="s">
-        <v>304</v>
+        <v>317</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>303</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
@@ -6407,10 +6407,10 @@
         <v>130</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>319</v>
-      </c>
-      <c r="D25" s="42" t="s">
-        <v>282</v>
+        <v>318</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>281</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
@@ -6426,10 +6426,10 @@
         <v>132</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>320</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>282</v>
+        <v>319</v>
+      </c>
+      <c r="D26" s="39" t="s">
+        <v>281</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
@@ -6445,10 +6445,10 @@
         <v>134</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>321</v>
-      </c>
-      <c r="D27" s="42" t="s">
-        <v>282</v>
+        <v>320</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>281</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
@@ -6464,10 +6464,10 @@
         <v>136</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>322</v>
-      </c>
-      <c r="D28" s="42" t="s">
-        <v>282</v>
+        <v>321</v>
+      </c>
+      <c r="D28" s="39" t="s">
+        <v>281</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
@@ -6485,7 +6485,7 @@
       <c r="C29" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="39" t="s">
         <v>16</v>
       </c>
       <c r="E29" s="17"/>
@@ -6504,7 +6504,7 @@
       <c r="C30" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="D30" s="42" t="s">
+      <c r="D30" s="39" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="17"/>
@@ -6523,7 +6523,7 @@
       <c r="C31" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="33" t="s">
         <v>16</v>
       </c>
       <c r="E31" s="17"/>
@@ -6538,7 +6538,7 @@
       <c r="C32" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="D32" s="36" t="s">
+      <c r="D32" s="33" t="s">
         <v>16</v>
       </c>
       <c r="E32" s="17"/>
@@ -6553,7 +6553,7 @@
       <c r="C33" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="D33" s="36" t="s">
+      <c r="D33" s="33" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="17"/>
@@ -6586,7 +6586,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6603,26 +6603,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="33" t="s">
-        <v>200</v>
-      </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="A2" s="41" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
@@ -6635,7 +6635,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -6655,15 +6655,15 @@
         <v>145</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" s="35" t="s">
+        <v>323</v>
+      </c>
+      <c r="D4" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="345" x14ac:dyDescent="0.15">
@@ -6674,15 +6674,15 @@
         <v>146</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>262</v>
-      </c>
-      <c r="D5" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="84" x14ac:dyDescent="0.15">
@@ -6693,9 +6693,9 @@
         <v>147</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="D6" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="17"/>
@@ -6712,9 +6712,9 @@
         <v>149</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="D7" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="17"/>
@@ -6731,9 +6731,9 @@
         <v>151</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="D8" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="17"/>
@@ -6750,9 +6750,9 @@
         <v>153</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="D9" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="17"/>
@@ -6802,26 +6802,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
@@ -6834,7 +6834,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -6856,7 +6856,7 @@
       <c r="C4" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="38" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="12"/>
@@ -6873,9 +6873,9 @@
         <v>159</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="D5" s="41" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" s="38" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="17"/>
@@ -6892,15 +6892,15 @@
         <v>161</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="D6" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="D6" s="38" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="70" x14ac:dyDescent="0.15">
@@ -6911,9 +6911,9 @@
         <v>162</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="D7" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" s="38" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="17"/>
@@ -6927,18 +6927,18 @@
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="D8" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="D8" s="38" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28" x14ac:dyDescent="0.15">
@@ -6946,18 +6946,18 @@
         <v>6</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="D9" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="D9" s="38" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="42" x14ac:dyDescent="0.15">
@@ -6968,9 +6968,9 @@
         <v>164</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="D10" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="38" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="17"/>
@@ -6987,9 +6987,9 @@
         <v>166</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D11" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="D11" s="38" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="17"/>

</xml_diff>

<commit_message>
add checklist on JWT
</commit_message>
<xml_diff>
--- a/Secure D Web Application Security Test Checklist v1.00.xlsx
+++ b/Secure D Web Application Security Test Checklist v1.00.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bankde/Desktop/work/wastc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C57E0C-E396-744A-B6FC-B3DA35007968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942495F5-A233-4745-8248-6F486C492293}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="327">
   <si>
     <t>Project Information</t>
   </si>
@@ -1316,28 +1316,6 @@
         <family val="1"/>
       </rPr>
       <t>https://www.owasp.org/index.php/Testing_for_cookies_attributes_(OTG-SESS-002)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Incorrect use of cookie or token
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>- Should not store any sensitive information in cleartext in a cookie.</t>
     </r>
   </si>
   <si>
@@ -3003,6 +2981,60 @@
 - Repeatable of discount, reward, voucher or gift.
 - Game with rewards or leaderboard from repetitive tasks (thus, vulnerable to bot) or client-side logic.
 - Signup reward of unauthenticated registration.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Incorrect use of cookie or token
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>- Should not store any sensitive information in cleartext in a cookie or token.</t>
+    </r>
+  </si>
+  <si>
+    <t>jwt.io
+c-jwt-cracker</t>
+  </si>
+  <si>
+    <r>
+      <t>Improper JWT implementation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+- Create and sign on the server side.
+- Use up-to-date or implement secure JWT interpreter.
+    - Do NOT accept "None" algorithm.
+    - Signature MUST be verified before processing.
+    - Strictly check the expiration (exp) payload.
+    - Not vulnerable against algorithm/key confusion (Change RS256 to HS256)
+- HMAC key MUST be larger than 256 bits.
+- Token validation MUST be unique, per-service keys.
+- Token should be revocable by both client and server.</t>
+    </r>
+  </si>
+  <si>
+    <t>Application MUST ensure that it uses secure and up-to-date JWT validation library. Signing MUST be performed on trusted server and the signing secret MUST be strong (HMAC key MUST be larger than 256 bits) and secure.
+Recommendation for JWT:
+https://cheatsheetseries.owasp.org/cheatsheets/JSON_Web_Token_for_Java_Cheat_Sheet.html</t>
   </si>
 </sst>
 </file>
@@ -3281,7 +3313,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3410,6 +3442,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4574,7 +4609,7 @@
   <dimension ref="A1:IV8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4630,7 +4665,7 @@
     <row r="8" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5"/>
       <c r="B8" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -4705,7 +4740,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -4725,10 +4760,10 @@
         <v>15</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D4" s="35" t="s">
         <v>268</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>269</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -4744,10 +4779,10 @@
         <v>168</v>
       </c>
       <c r="C5" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>270</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>271</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -4763,10 +4798,10 @@
         <v>17</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -4782,10 +4817,10 @@
         <v>18</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
@@ -4801,10 +4836,10 @@
         <v>20</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -4820,10 +4855,10 @@
         <v>22</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
@@ -4854,7 +4889,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>169</v>
@@ -4873,10 +4908,10 @@
         <v>27</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
@@ -4892,10 +4927,10 @@
         <v>225</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -4976,7 +5011,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -4996,10 +5031,10 @@
         <v>31</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -5015,10 +5050,10 @@
         <v>33</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -5075,7 +5110,7 @@
         <v>227</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -5103,10 +5138,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D10" s="37" t="s">
         <v>16</v>
@@ -5125,7 +5160,7 @@
         <v>39</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D11" s="37" t="s">
         <v>16</v>
@@ -5144,7 +5179,7 @@
         <v>41</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D12" s="37" t="s">
         <v>16</v>
@@ -5163,10 +5198,10 @@
         <v>43</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -5182,10 +5217,10 @@
         <v>45</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
@@ -5197,10 +5232,10 @@
       <c r="A15" s="14"/>
       <c r="B15" s="26"/>
       <c r="C15" s="22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
@@ -5216,10 +5251,10 @@
         <v>47</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
@@ -5235,10 +5270,10 @@
         <v>48</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
@@ -5254,10 +5289,10 @@
         <v>50</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -5273,10 +5308,10 @@
         <v>52</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -5307,10 +5342,10 @@
         <v>54</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
@@ -5326,10 +5361,10 @@
         <v>55</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
@@ -5342,10 +5377,10 @@
         <v>17</v>
       </c>
       <c r="B23" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>264</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>265</v>
       </c>
       <c r="D23" s="37" t="s">
         <v>16</v>
@@ -5353,7 +5388,7 @@
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -5374,13 +5409,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IW31"/>
+  <dimension ref="A1:IW32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5429,7 +5464,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -5702,7 +5737,7 @@
       <c r="A19" s="20"/>
       <c r="B19" s="26"/>
       <c r="C19" s="22" t="s">
-        <v>244</v>
+        <v>323</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>16</v>
@@ -5713,30 +5748,30 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="140" x14ac:dyDescent="0.15">
-      <c r="A20" s="14">
-        <v>9</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>245</v>
+    <row r="20" spans="1:7" ht="154" x14ac:dyDescent="0.15">
+      <c r="A20" s="20"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="43" t="s">
+        <v>325</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>16</v>
+        <v>324</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="70" x14ac:dyDescent="0.15">
-      <c r="A21" s="20"/>
-      <c r="B21" s="26"/>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="140" x14ac:dyDescent="0.15">
+      <c r="A21" s="14">
+        <v>9</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>79</v>
+      </c>
       <c r="C21" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D21" s="32" t="s">
         <v>16</v>
@@ -5744,48 +5779,44 @@
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="112" x14ac:dyDescent="0.15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="70" x14ac:dyDescent="0.15">
       <c r="A22" s="20"/>
       <c r="B22" s="26"/>
       <c r="C22" s="22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D22" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
-      <c r="G22" s="24" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="56" x14ac:dyDescent="0.15">
+      <c r="G22" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="112" x14ac:dyDescent="0.15">
       <c r="A23" s="20"/>
       <c r="B23" s="26"/>
       <c r="C23" s="22" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D23" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
-      <c r="G23" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="126" x14ac:dyDescent="0.15">
-      <c r="A24" s="14">
-        <v>10</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>83</v>
-      </c>
+      <c r="G23" s="24" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="56" x14ac:dyDescent="0.15">
+      <c r="A24" s="20"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D24" s="32" t="s">
         <v>16</v>
@@ -5793,14 +5824,18 @@
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="70" x14ac:dyDescent="0.15">
-      <c r="A25" s="20"/>
-      <c r="B25" s="26"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="126" x14ac:dyDescent="0.15">
+      <c r="A25" s="14">
+        <v>10</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>83</v>
+      </c>
       <c r="C25" s="22" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D25" s="32" t="s">
         <v>16</v>
@@ -5808,18 +5843,14 @@
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
       <c r="G25" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="56" x14ac:dyDescent="0.15">
-      <c r="A26" s="14">
-        <v>11</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>216</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+      <c r="A26" s="20"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="22" t="s">
+        <v>250</v>
       </c>
       <c r="D26" s="32" t="s">
         <v>16</v>
@@ -5827,18 +5858,18 @@
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="112" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="56" x14ac:dyDescent="0.15">
       <c r="A27" s="14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>178</v>
+        <v>216</v>
       </c>
       <c r="D27" s="32" t="s">
         <v>16</v>
@@ -5846,18 +5877,18 @@
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
       <c r="G27" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="112" x14ac:dyDescent="0.15">
       <c r="A28" s="14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D28" s="32" t="s">
         <v>16</v>
@@ -5865,56 +5896,56 @@
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
       <c r="G28" s="18" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="126" x14ac:dyDescent="0.15">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="112" x14ac:dyDescent="0.15">
       <c r="A29" s="14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D29" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
-      <c r="G29" s="24" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+      <c r="G29" s="18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="126" x14ac:dyDescent="0.15">
       <c r="A30" s="14">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D30" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
-      <c r="G30" s="18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="84" x14ac:dyDescent="0.15">
+      <c r="G30" s="24" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="70" x14ac:dyDescent="0.15">
       <c r="A31" s="14">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D31" s="32" t="s">
         <v>16</v>
@@ -5922,6 +5953,25 @@
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
       <c r="G31" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="84" x14ac:dyDescent="0.15">
+      <c r="A32" s="14">
+        <v>16</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="18" t="s">
         <v>95</v>
       </c>
     </row>
@@ -5998,7 +6048,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -6018,15 +6068,15 @@
         <v>98</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="126" x14ac:dyDescent="0.15">
@@ -6037,10 +6087,10 @@
         <v>99</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -6056,10 +6106,10 @@
         <v>101</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -6075,10 +6125,10 @@
         <v>103</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
@@ -6094,10 +6144,10 @@
         <v>105</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -6113,10 +6163,10 @@
         <v>107</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
@@ -6132,7 +6182,7 @@
         <v>108</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="17"/>
@@ -6149,22 +6199,22 @@
         <v>110</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="70" x14ac:dyDescent="0.15">
       <c r="A12" s="20"/>
       <c r="B12" s="26"/>
       <c r="C12" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D12" s="39" t="s">
         <v>16</v>
@@ -6179,10 +6229,10 @@
       <c r="A13" s="20"/>
       <c r="B13" s="26"/>
       <c r="C13" s="22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -6217,10 +6267,10 @@
         <v>115</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
@@ -6236,10 +6286,10 @@
         <v>116</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
@@ -6255,7 +6305,7 @@
         <v>117</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D17" s="33" t="s">
         <v>16</v>
@@ -6274,10 +6324,10 @@
         <v>119</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -6293,10 +6343,10 @@
         <v>121</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -6350,7 +6400,7 @@
         <v>126</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D22" s="33" t="s">
         <v>16</v>
@@ -6369,7 +6419,7 @@
         <v>223</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D23" s="33" t="s">
         <v>16</v>
@@ -6388,10 +6438,10 @@
         <v>128</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
@@ -6407,10 +6457,10 @@
         <v>130</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
@@ -6426,10 +6476,10 @@
         <v>132</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
@@ -6445,10 +6495,10 @@
         <v>134</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
@@ -6464,10 +6514,10 @@
         <v>136</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
@@ -6635,7 +6685,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -6655,7 +6705,7 @@
         <v>145</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>16</v>
@@ -6674,7 +6724,7 @@
         <v>146</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>16</v>
@@ -6834,7 +6884,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
rephrase on HTTP pollution
</commit_message>
<xml_diff>
--- a/Secure D Web Application Security Test Checklist v1.00.xlsx
+++ b/Secure D Web Application Security Test Checklist v1.00.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bankde/Desktop/work/wastc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9464252E-28A9-8748-94B5-7961569A5D8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4E5F22-7818-C743-BCF9-B5F3C3F0BC89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,12 +482,6 @@
     <t>HTTP parameter / Json / XML pollution</t>
   </si>
   <si>
-    <t>[CWE-235]
-Developer should process the user input through the framework method so the inputs from HTTP parameters are always consistent.
-Developer MUST carefully study the framework how it processes the HTTP parameter.
-For frontend javascript, do NOT manually concatenate the user input into a server request, using framework request form is recommended.</t>
-  </si>
-  <si>
     <t>HTTP methods tampering</t>
   </si>
   <si>
@@ -1628,56 +1622,6 @@
         <family val="1"/>
       </rPr>
       <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">- String concatenation without escape of control characters on client side.
-    - HTTP &amp; = % #
-    - JSON " ' , { } \
-    - XML &lt; &gt; /
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Improper handling of duplicate key/input parameter.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>The application should NEVER interpret multiple values of the same key/parameter. Accepting multiple values as array could lead to input validation bypass.
-- The application MUST be consistent whether to use first occurrence or the latter in the whole process. The issue will occur if application validates on first occurrence but actual operation uses the second.
-- The application can decide to reject malicious or malformed requests.</t>
     </r>
   </si>
   <si>
@@ -3051,6 +2995,63 @@
     <t>Ensure that your application's JWT validation library is secure and updated to secure version. Signing MUST be performed on trusted server and the signing secret MUST be strong (HMAC key MUST be larger than 256 bits) and secure.
 Recommendation for JWT:
 https://cheatsheetseries.owasp.org/cheatsheets/JSON_Web_Token_for_Java_Cheat_Sheet.html</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- String concatenation without escape of control characters during the parameters, JSON, or XML creation. This may happen on either client or server side.
+    - HTTP &amp; = % #
+    - JSON " ' , { } \
+    - XML &lt; &gt; /
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Improper handling of duplicate key/input parameter.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>The application should NEVER interpret multiple values of the same key/parameter. Accepting multiple values as array could lead to input validation bypass.
+- The application MUST be consistent whether to use first occurrence or the latter in the whole process. The issue will occur if application validates on first occurrence but actual operation uses the second.
+- The application can decide to reject malicious or malformed requests.</t>
+    </r>
+  </si>
+  <si>
+    <t>[CWE-235]
+Developer should process the user input through the framework method so the inputs from HTTP parameters are always consistent.
+Developer MUST carefully study the framework how it processes the HTTP parameter.
+Do NOT manually concatenate the user input into a server request, JSON, or XML creation. For frontend developer, using framework request form is recommended. For backend developer, using secure template is recommended.
+The developer could carefully study the control characters and manually escape them before HTTP requests, JSON, or XML creation. The control characters can be varied and can be easily missed. This option should only be done when there is no other solutions.</t>
   </si>
 </sst>
 </file>
@@ -4625,7 +4626,7 @@
   <dimension ref="A1:IV8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4681,7 +4682,7 @@
     <row r="8" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5"/>
       <c r="B8" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -4756,7 +4757,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -4776,10 +4777,10 @@
         <v>15</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -4792,13 +4793,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -4814,10 +4815,10 @@
         <v>17</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -4833,10 +4834,10 @@
         <v>18</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
@@ -4852,10 +4853,10 @@
         <v>20</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -4871,10 +4872,10 @@
         <v>22</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
@@ -4905,15 +4906,15 @@
         <v>26</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="42" x14ac:dyDescent="0.15">
@@ -4924,10 +4925,10 @@
         <v>27</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
@@ -4940,18 +4941,18 @@
         <v>9</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
       <c r="G13" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -5027,7 +5028,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -5047,10 +5048,10 @@
         <v>31</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -5066,10 +5067,10 @@
         <v>33</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -5082,10 +5083,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>208</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>209</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>16</v>
@@ -5093,7 +5094,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="84" x14ac:dyDescent="0.15">
@@ -5104,7 +5105,7 @@
         <v>35</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>16</v>
@@ -5123,22 +5124,22 @@
         <v>37</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="70" x14ac:dyDescent="0.15">
       <c r="A9" s="14"/>
       <c r="B9" s="26"/>
       <c r="C9" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>16</v>
@@ -5146,7 +5147,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="154" x14ac:dyDescent="0.15">
@@ -5154,10 +5155,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D10" s="37" t="s">
         <v>16</v>
@@ -5176,7 +5177,7 @@
         <v>39</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D11" s="37" t="s">
         <v>16</v>
@@ -5195,7 +5196,7 @@
         <v>41</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D12" s="37" t="s">
         <v>16</v>
@@ -5214,10 +5215,10 @@
         <v>43</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -5233,10 +5234,10 @@
         <v>45</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
@@ -5248,15 +5249,15 @@
       <c r="A15" s="14"/>
       <c r="B15" s="26"/>
       <c r="C15" s="22" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
       <c r="G15" s="24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="140" x14ac:dyDescent="0.15">
@@ -5267,15 +5268,15 @@
         <v>47</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="84" x14ac:dyDescent="0.15">
@@ -5286,10 +5287,10 @@
         <v>48</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
@@ -5305,10 +5306,10 @@
         <v>50</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -5324,10 +5325,10 @@
         <v>52</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -5339,7 +5340,7 @@
       <c r="A20" s="27"/>
       <c r="B20" s="23"/>
       <c r="C20" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D20" s="37" t="s">
         <v>16</v>
@@ -5358,15 +5359,15 @@
         <v>54</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="56" x14ac:dyDescent="0.15">
@@ -5377,10 +5378,10 @@
         <v>55</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
@@ -5393,10 +5394,10 @@
         <v>17</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D23" s="37" t="s">
         <v>16</v>
@@ -5404,7 +5405,7 @@
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -5480,7 +5481,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -5500,7 +5501,7 @@
         <v>59</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>16</v>
@@ -5508,7 +5509,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="126" x14ac:dyDescent="0.15">
@@ -5519,7 +5520,7 @@
         <v>60</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>16</v>
@@ -5527,14 +5528,14 @@
       <c r="E5" s="12"/>
       <c r="F5" s="17"/>
       <c r="G5" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="70" x14ac:dyDescent="0.15">
       <c r="A6" s="20"/>
       <c r="B6" s="26"/>
       <c r="C6" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>16</v>
@@ -5549,7 +5550,7 @@
       <c r="A7" s="20"/>
       <c r="B7" s="26"/>
       <c r="C7" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>16</v>
@@ -5568,7 +5569,7 @@
         <v>63</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>16</v>
@@ -5583,7 +5584,7 @@
       <c r="A9" s="20"/>
       <c r="B9" s="26"/>
       <c r="C9" s="22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>16</v>
@@ -5598,7 +5599,7 @@
       <c r="A10" s="20"/>
       <c r="B10" s="26"/>
       <c r="C10" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>16</v>
@@ -5613,7 +5614,7 @@
       <c r="A11" s="20"/>
       <c r="B11" s="26"/>
       <c r="C11" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D11" s="32" t="s">
         <v>16</v>
@@ -5628,7 +5629,7 @@
       <c r="A12" s="20"/>
       <c r="B12" s="26"/>
       <c r="C12" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D12" s="32" t="s">
         <v>16</v>
@@ -5647,7 +5648,7 @@
         <v>69</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D13" s="32" t="s">
         <v>16</v>
@@ -5666,7 +5667,7 @@
         <v>71</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D14" s="32" t="s">
         <v>16</v>
@@ -5685,7 +5686,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D15" s="32" t="s">
         <v>16</v>
@@ -5704,7 +5705,7 @@
         <v>75</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D16" s="32" t="s">
         <v>16</v>
@@ -5723,7 +5724,7 @@
         <v>77</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D17" s="32" t="s">
         <v>16</v>
@@ -5731,14 +5732,14 @@
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
       <c r="G17" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="42" x14ac:dyDescent="0.15">
       <c r="A18" s="20"/>
       <c r="B18" s="26"/>
       <c r="C18" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D18" s="32" t="s">
         <v>16</v>
@@ -5746,14 +5747,14 @@
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="84" x14ac:dyDescent="0.15">
       <c r="A19" s="20"/>
       <c r="B19" s="26"/>
       <c r="C19" s="22" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>16</v>
@@ -5768,15 +5769,15 @@
       <c r="A20" s="20"/>
       <c r="B20" s="26"/>
       <c r="C20" s="40" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="18" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="140" x14ac:dyDescent="0.15">
@@ -5787,7 +5788,7 @@
         <v>79</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D21" s="32" t="s">
         <v>16</v>
@@ -5802,7 +5803,7 @@
       <c r="A22" s="20"/>
       <c r="B22" s="26"/>
       <c r="C22" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D22" s="32" t="s">
         <v>16</v>
@@ -5817,7 +5818,7 @@
       <c r="A23" s="20"/>
       <c r="B23" s="26"/>
       <c r="C23" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D23" s="32" t="s">
         <v>16</v>
@@ -5825,14 +5826,14 @@
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="56" x14ac:dyDescent="0.15">
       <c r="A24" s="20"/>
       <c r="B24" s="26"/>
       <c r="C24" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D24" s="32" t="s">
         <v>16</v>
@@ -5851,7 +5852,7 @@
         <v>83</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D25" s="32" t="s">
         <v>16</v>
@@ -5866,7 +5867,7 @@
       <c r="A26" s="20"/>
       <c r="B26" s="26"/>
       <c r="C26" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D26" s="32" t="s">
         <v>16</v>
@@ -5885,7 +5886,7 @@
         <v>86</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D27" s="32" t="s">
         <v>16</v>
@@ -5904,7 +5905,7 @@
         <v>88</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D28" s="32" t="s">
         <v>16</v>
@@ -5923,7 +5924,7 @@
         <v>90</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D29" s="32" t="s">
         <v>16</v>
@@ -5931,7 +5932,7 @@
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
       <c r="G29" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="126" x14ac:dyDescent="0.15">
@@ -5942,7 +5943,7 @@
         <v>91</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D30" s="32" t="s">
         <v>16</v>
@@ -5950,7 +5951,7 @@
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
       <c r="G30" s="24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="70" x14ac:dyDescent="0.15">
@@ -5961,7 +5962,7 @@
         <v>92</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D31" s="32" t="s">
         <v>16</v>
@@ -5980,7 +5981,7 @@
         <v>94</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D32" s="32" t="s">
         <v>16</v>
@@ -6064,7 +6065,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -6084,15 +6085,15 @@
         <v>98</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="126" x14ac:dyDescent="0.15">
@@ -6103,10 +6104,10 @@
         <v>99</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -6122,10 +6123,10 @@
         <v>101</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -6141,10 +6142,10 @@
         <v>103</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
@@ -6160,10 +6161,10 @@
         <v>105</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -6179,15 +6180,15 @@
         <v>107</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="182" x14ac:dyDescent="0.15">
@@ -6198,7 +6199,7 @@
         <v>108</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="17"/>
@@ -6215,22 +6216,22 @@
         <v>110</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="70" x14ac:dyDescent="0.15">
       <c r="A12" s="20"/>
       <c r="B12" s="26"/>
       <c r="C12" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D12" s="39" t="s">
         <v>16</v>
@@ -6245,10 +6246,10 @@
       <c r="A13" s="20"/>
       <c r="B13" s="26"/>
       <c r="C13" s="22" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -6264,7 +6265,7 @@
         <v>113</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D14" s="33" t="s">
         <v>16</v>
@@ -6283,15 +6284,15 @@
         <v>115</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
       <c r="G15" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="154" x14ac:dyDescent="0.15">
@@ -6302,15 +6303,15 @@
         <v>116</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="98" x14ac:dyDescent="0.15">
@@ -6321,7 +6322,7 @@
         <v>117</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D17" s="33" t="s">
         <v>16</v>
@@ -6340,10 +6341,10 @@
         <v>119</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -6359,15 +6360,15 @@
         <v>121</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="168" x14ac:dyDescent="0.15">
@@ -6378,7 +6379,7 @@
         <v>122</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D20" s="33" t="s">
         <v>16</v>
@@ -6397,7 +6398,7 @@
         <v>124</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D21" s="33" t="s">
         <v>16</v>
@@ -6408,7 +6409,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="210" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="252" x14ac:dyDescent="0.15">
       <c r="A22" s="14">
         <v>16</v>
       </c>
@@ -6416,7 +6417,7 @@
         <v>126</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>258</v>
+        <v>328</v>
       </c>
       <c r="D22" s="33" t="s">
         <v>16</v>
@@ -6424,7 +6425,7 @@
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="18" t="s">
-        <v>127</v>
+        <v>329</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="168" x14ac:dyDescent="0.15">
@@ -6432,16 +6433,16 @@
         <v>17</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D23" s="33"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="18" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="84" x14ac:dyDescent="0.15">
@@ -6449,10 +6450,10 @@
         <v>18</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D24" s="33" t="s">
         <v>16</v>
@@ -6460,7 +6461,7 @@
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="98" x14ac:dyDescent="0.15">
@@ -6468,18 +6469,18 @@
         <v>19</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
       <c r="G25" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="98" x14ac:dyDescent="0.15">
@@ -6487,18 +6488,18 @@
         <v>20</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="98" x14ac:dyDescent="0.15">
@@ -6506,18 +6507,18 @@
         <v>21</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
       <c r="G27" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="98" x14ac:dyDescent="0.15">
@@ -6525,18 +6526,18 @@
         <v>22</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
       <c r="G28" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="140" x14ac:dyDescent="0.15">
@@ -6544,18 +6545,18 @@
         <v>23</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
       <c r="G29" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="210" x14ac:dyDescent="0.15">
@@ -6563,10 +6564,10 @@
         <v>24</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D30" s="39" t="s">
         <v>16</v>
@@ -6574,7 +6575,7 @@
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
       <c r="G30" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="112" x14ac:dyDescent="0.15">
@@ -6582,10 +6583,10 @@
         <v>25</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D31" s="39" t="s">
         <v>16</v>
@@ -6593,7 +6594,7 @@
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
       <c r="G31" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="70" x14ac:dyDescent="0.15">
@@ -6601,10 +6602,10 @@
         <v>26</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D32" s="33" t="s">
         <v>16</v>
@@ -6612,14 +6613,14 @@
       <c r="E32" s="17"/>
       <c r="F32" s="17"/>
       <c r="G32" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A33" s="20"/>
       <c r="B33" s="26"/>
       <c r="C33" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D33" s="33" t="s">
         <v>16</v>
@@ -6627,14 +6628,14 @@
       <c r="E33" s="17"/>
       <c r="F33" s="17"/>
       <c r="G33" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="84" x14ac:dyDescent="0.15">
       <c r="A34" s="20"/>
       <c r="B34" s="26"/>
       <c r="C34" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D34" s="33" t="s">
         <v>16</v>
@@ -6687,7 +6688,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
@@ -6698,7 +6699,7 @@
     </row>
     <row r="2" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
@@ -6718,7 +6719,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -6735,10 +6736,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>16</v>
@@ -6746,7 +6747,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="345" x14ac:dyDescent="0.15">
@@ -6754,10 +6755,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>16</v>
@@ -6765,7 +6766,7 @@
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="84" x14ac:dyDescent="0.15">
@@ -6773,10 +6774,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>16</v>
@@ -6784,7 +6785,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="112" x14ac:dyDescent="0.15">
@@ -6792,10 +6793,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>16</v>
@@ -6803,7 +6804,7 @@
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="84" x14ac:dyDescent="0.15">
@@ -6811,10 +6812,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>16</v>
@@ -6822,7 +6823,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="70" x14ac:dyDescent="0.15">
@@ -6830,10 +6831,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>16</v>
@@ -6841,7 +6842,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -6886,7 +6887,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.15">
       <c r="A1" s="41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
@@ -6897,7 +6898,7 @@
     </row>
     <row r="2" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
@@ -6917,7 +6918,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -6934,10 +6935,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>16</v>
@@ -6945,7 +6946,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="42" x14ac:dyDescent="0.15">
@@ -6953,10 +6954,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D5" s="38" t="s">
         <v>16</v>
@@ -6964,7 +6965,7 @@
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="56" x14ac:dyDescent="0.15">
@@ -6972,10 +6973,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D6" s="38" t="s">
         <v>16</v>
@@ -6983,7 +6984,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="70" x14ac:dyDescent="0.15">
@@ -6991,10 +6992,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7" s="38" t="s">
         <v>16</v>
@@ -7002,7 +7003,7 @@
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28" x14ac:dyDescent="0.15">
@@ -7010,10 +7011,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D8" s="38" t="s">
         <v>16</v>
@@ -7021,7 +7022,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28" x14ac:dyDescent="0.15">
@@ -7029,10 +7030,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D9" s="38" t="s">
         <v>16</v>
@@ -7040,7 +7041,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="42" x14ac:dyDescent="0.15">
@@ -7048,10 +7049,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D10" s="38" t="s">
         <v>16</v>
@@ -7059,7 +7060,7 @@
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="56" x14ac:dyDescent="0.15">
@@ -7067,10 +7068,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D11" s="38" t="s">
         <v>16</v>
@@ -7078,7 +7079,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>